<commit_message>
Add handling of multiple projects to td2cambio
</commit_message>
<xml_diff>
--- a/Cambio-mall.xlsx
+++ b/Cambio-mall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.nilefalk\Utveckling\td2tlu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.nilefalk\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2CA46A-AB22-4DDC-8ACA-51725B3867BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{507A49ED-39CC-4259-A155-65A0612CA426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9720" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4200" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Konsulttidrapport" sheetId="1" r:id="rId1"/>
@@ -539,23 +539,23 @@
   </sheetPr>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -574,7 +574,7 @@
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -595,7 +595,7 @@
       <c r="N2" s="18"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -616,7 +616,7 @@
       <c r="N3" s="10"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -637,7 +637,7 @@
       <c r="N4" s="19"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -658,7 +658,7 @@
       <c r="N5" s="18"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -679,7 +679,7 @@
       <c r="N6" s="18"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -708,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43862</v>
       </c>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43863</v>
       </c>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43864</v>
       </c>
@@ -774,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43865</v>
       </c>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43866</v>
       </c>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43867</v>
       </c>
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43868</v>
       </c>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43869</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43870</v>
       </c>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43871</v>
       </c>
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43872</v>
       </c>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43873</v>
       </c>
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43874</v>
       </c>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43875</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="Q21" s="12"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43876</v>
       </c>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="Q22" s="12"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43877</v>
       </c>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="Q23" s="12"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43878</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43879</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43880</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43881</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43882</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43883</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43884</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43885</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43886</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43887</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43888</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43889</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43890</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43891</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43892</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
@@ -1401,21 +1401,57 @@
         <f>SUM(B8:B38)</f>
         <v>0</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
+      <c r="C39" s="11">
+        <f t="shared" ref="C39:N39" si="1">SUM(C8:C38)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O39" s="7"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1458,9 +1494,9 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1510,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -1486,7 +1522,7 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C7" s="13" t="s">
         <v>9</v>
       </c>
@@ -1500,7 +1536,7 @@
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C8" s="13" t="s">
         <v>14</v>
       </c>
@@ -1514,7 +1550,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C9" s="13" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1564,7 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1542,7 +1578,7 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -1556,7 +1592,7 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
@@ -1570,7 +1606,7 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C13" s="13" t="s">
         <v>15</v>
       </c>
@@ -1584,7 +1620,7 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -1596,7 +1632,7 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1608,7 +1644,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1620,7 +1656,7 @@
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C17" s="14" t="s">
         <v>16</v>
       </c>
@@ -1634,7 +1670,7 @@
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="14"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -1646,7 +1682,7 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="14" t="s">
         <v>17</v>
       </c>
@@ -1660,7 +1696,7 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>

</xml_diff>